<commit_message>
fixed negative prices and 1.2
</commit_message>
<xml_diff>
--- a/data/Price_dayahead.xlsx
+++ b/data/Price_dayahead.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loict\OneDrive\Skrivebord\Jalal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tgilh\git_master_laptop\46755\46755_2_ass\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22C827CC-DE62-4703-B63B-6DFD78DA4AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6C1C6F-64EA-4615-9CCB-AEED6CEFA2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="1008" windowWidth="21600" windowHeight="11232" xr2:uid="{1D41FAD5-2774-4139-92D9-CC6CC448654F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{1D41FAD5-2774-4139-92D9-CC6CC448654F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -551,14 +551,16 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -623,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +690,7 @@
         <v>128.19999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -753,7 +755,7 @@
         <v>120.38</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -818,7 +820,7 @@
         <v>117.09</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -883,7 +885,7 @@
         <v>112.15</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -948,7 +950,7 @@
         <v>109.75</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1015,7 @@
         <v>111.89</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1078,7 +1080,7 @@
         <v>117.11</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>135.81</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1210,7 @@
         <v>138.82</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1273,7 +1275,7 @@
         <v>137.77000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1338,7 +1340,7 @@
         <v>125.08</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1388,7 +1390,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="Q13" s="7">
-        <v>-0.67</v>
+        <v>0</v>
       </c>
       <c r="R13" s="6">
         <v>13.26</v>
@@ -1403,7 +1405,7 @@
         <v>112.1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1411,10 +1413,10 @@
         <v>3.13</v>
       </c>
       <c r="C14" s="8">
-        <v>-0.56000000000000005</v>
+        <v>0</v>
       </c>
       <c r="D14" s="8">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3">
         <v>31.14</v>
@@ -1444,7 +1446,7 @@
         <v>1.29</v>
       </c>
       <c r="N14" s="8">
-        <v>-0.33</v>
+        <v>0</v>
       </c>
       <c r="O14" s="2">
         <v>13.08</v>
@@ -1453,7 +1455,7 @@
         <v>0.08</v>
       </c>
       <c r="Q14" s="8">
-        <v>-0.7</v>
+        <v>0</v>
       </c>
       <c r="R14" s="3">
         <v>4</v>
@@ -1468,7 +1470,7 @@
         <v>102.21</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1476,10 +1478,10 @@
         <v>3.41</v>
       </c>
       <c r="C15" s="7">
-        <v>-0.16</v>
+        <v>0</v>
       </c>
       <c r="D15" s="7">
-        <v>-0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="E15" s="6">
         <v>27.92</v>
@@ -1509,7 +1511,7 @@
         <v>3.95</v>
       </c>
       <c r="N15" s="7">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="O15" s="5">
         <v>8.08</v>
@@ -1518,7 +1520,7 @@
         <v>0.02</v>
       </c>
       <c r="Q15" s="7">
-        <v>-0.78</v>
+        <v>0</v>
       </c>
       <c r="R15" s="6">
         <v>4.04</v>
@@ -1533,7 +1535,7 @@
         <v>97.27</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1598,7 +1600,7 @@
         <v>99.39</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1663,7 +1665,7 @@
         <v>97.8</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1728,7 +1730,7 @@
         <v>125.41</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1793,7 +1795,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1858,7 +1860,7 @@
         <v>158.55000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
@@ -1923,7 +1925,7 @@
         <v>150.78</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1988,7 +1990,7 @@
         <v>133.41</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -2053,7 +2055,7 @@
         <v>125.42</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2118,7 +2120,7 @@
         <v>122.03</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
@@ -2183,76 +2185,76 @@
         <v>119.9</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A49" s="4"/>
     </row>
-    <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A53" s="4"/>
     </row>
   </sheetData>

</xml_diff>